<commit_message>
[FIX] fix gitlab password message template
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/init-data/hzero_message/hzero_message/hzero-data-message-template-open.xlsx
+++ b/src/main/resources/script/db/init-data/hzero_message/hzero_message/hzero-data-message-template-open.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420" tabRatio="597" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12855" tabRatio="597" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -3306,7 +3306,135 @@
     <t>GitLab默认密码</t>
   </si>
   <si>
-    <t>您的GitLab仓库密码为: ${gitlabPassword}。为了您的账户安全，请尽快前往Choerodon&lt;a href='#/iam/user-info?type=site&amp;organizationId=${organizationId}'&gt;个人信息&lt;/a&gt;页面修改默认的GitLab密码</t>
+    <r>
+      <t>您的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="134"/>
+      </rPr>
+      <t>GitLab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>仓库密码为</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="134"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="134"/>
+      </rPr>
+      <t>${gitlabPassword}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>。为了您的账户安全，请尽快前往</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Choerodon&lt;a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="134"/>
+      </rPr>
+      <t>href='#/rducm/personal-setting?type=site&amp;organizationId=${organizationId}'&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>个人设置</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&lt;/a&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>页面修改默认的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <charset val="134"/>
+      </rPr>
+      <t>GitLab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>密码</t>
+    </r>
   </si>
   <si>
     <t>hmsg_message_template-70</t>
@@ -8051,12 +8179,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="41">
+  <fonts count="42">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -8114,6 +8242,12 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FFC55A11"/>
       <name val="DengXian"/>
       <charset val="134"/>
@@ -8131,59 +8265,100 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="DengXian"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -8191,29 +8366,37 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -8221,76 +8404,27 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF003366"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
       <charset val="134"/>
     </font>
     <font>
@@ -8370,7 +8504,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8382,49 +8630,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8436,31 +8666,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8472,85 +8684,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8567,12 +8701,28 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -8597,6 +8747,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -8605,26 +8768,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -8639,15 +8782,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -8657,17 +8791,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -8687,11 +8824,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -8703,21 +8846,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -8740,168 +8868,174 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -8916,10 +9050,10 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -8930,112 +9064,112 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="50">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
-    <cellStyle name="常规 2" xfId="49"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="常规 2" xfId="14"/>
+    <cellStyle name="Accent3" xfId="15" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="16" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="17" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="18" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="19" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="21" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="22" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="23" builtinId="32"/>
+    <cellStyle name="Bad" xfId="24" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="25" builtinId="42"/>
+    <cellStyle name="Total" xfId="26" builtinId="25"/>
+    <cellStyle name="Output" xfId="27" builtinId="21"/>
+    <cellStyle name="Currency" xfId="28" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="29" builtinId="38"/>
+    <cellStyle name="Note" xfId="30" builtinId="10"/>
+    <cellStyle name="Input" xfId="31" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="32" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="33" builtinId="22"/>
+    <cellStyle name="Good" xfId="34" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="35" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="36" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="37" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="38" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="41" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="42" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
+    <cellStyle name="Comma" xfId="45" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
@@ -9378,22 +9512,22 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="15.5694444444444" style="12" customWidth="1"/>
-    <col min="2" max="2" width="10.2847222222222" style="13" customWidth="1"/>
-    <col min="3" max="3" width="28.1388888888889" customWidth="1"/>
-    <col min="4" max="4" width="35.2847222222222" style="11" customWidth="1"/>
-    <col min="5" max="5" width="38.5694444444444" customWidth="1"/>
-    <col min="6" max="6" width="23.4236111111111" customWidth="1"/>
-    <col min="7" max="7" width="21.5694444444444" customWidth="1"/>
+    <col min="1" max="1" width="15.5666666666667" style="12" customWidth="1"/>
+    <col min="2" max="2" width="10.2866666666667" style="13" customWidth="1"/>
+    <col min="3" max="3" width="28.14" customWidth="1"/>
+    <col min="4" max="4" width="35.2866666666667" style="10" customWidth="1"/>
+    <col min="5" max="5" width="38.5666666666667" customWidth="1"/>
+    <col min="6" max="6" width="23.4266666666667" customWidth="1"/>
+    <col min="7" max="7" width="21.5666666666667" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="24.5694444444444" customWidth="1"/>
+    <col min="9" max="9" width="24.5666666666667" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="11" width="19.1388888888889" customWidth="1"/>
-    <col min="12" max="12" width="18.5694444444444" customWidth="1"/>
-    <col min="13" max="13" width="13.1388888888889" customWidth="1"/>
-    <col min="14" max="1025" width="10.2847222222222" customWidth="1"/>
+    <col min="11" max="11" width="19.14" customWidth="1"/>
+    <col min="12" max="12" width="18.5666666666667" customWidth="1"/>
+    <col min="13" max="13" width="13.14" customWidth="1"/>
+    <col min="14" max="1025" width="10.2866666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="64.5" customHeight="1" spans="1:8">
@@ -9403,130 +9537,130 @@
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="5:5">
-      <c r="E2" s="17"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" ht="49.5" customHeight="1" spans="3:7">
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="16"/>
+      <c r="E3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-    </row>
-    <row r="4" spans="3:7">
-      <c r="C4" s="20" t="s">
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+    </row>
+    <row r="4" ht="24" spans="3:7">
+      <c r="C4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21" t="s">
+      <c r="D4" s="17"/>
+      <c r="E4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" ht="24" spans="1:3">
       <c r="A5" s="14"/>
       <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="3:5">
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="37" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="3:5">
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="29"/>
-    </row>
-    <row r="9" ht="52.2" spans="3:6">
-      <c r="C9" s="30" t="s">
+      <c r="E8" s="38"/>
+    </row>
+    <row r="9" ht="72" spans="3:6">
+      <c r="C9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="39" t="s">
         <v>15</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" ht="52.2" spans="3:5">
-      <c r="C10" s="33" t="s">
+    <row r="10" ht="65.25" spans="3:5">
+      <c r="C10" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="39" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" ht="69.6" spans="3:5">
-      <c r="C11" s="27" t="s">
+    <row r="11" ht="96" spans="3:5">
+      <c r="C11" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="39" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="3:5">
-      <c r="C12" s="27" t="s">
+    <row r="12" ht="24" spans="3:5">
+      <c r="C12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="40" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="3:5">
-      <c r="C13" s="27"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="38"/>
     </row>
     <row r="14" spans="3:5">
-      <c r="C14" s="27"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="29"/>
-    </row>
-    <row r="15" ht="34.8" spans="3:5">
-      <c r="C15" s="35" t="s">
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="38"/>
+    </row>
+    <row r="15" ht="48" spans="3:5">
+      <c r="C15" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="37" t="s">
+      <c r="E15" s="41" t="s">
         <v>28</v>
       </c>
     </row>
@@ -9535,65 +9669,65 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="3:5">
-      <c r="C19" s="38" t="s">
+    <row r="19" ht="24" spans="3:5">
+      <c r="C19" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-    </row>
-    <row r="20" spans="3:4">
-      <c r="C20" s="39" t="s">
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+    </row>
+    <row r="20" ht="24" spans="3:4">
+      <c r="C20" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="3:4">
-      <c r="C21" s="39" t="s">
+    <row r="21" ht="24" spans="3:4">
+      <c r="C21" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="3:4">
-      <c r="C22" s="39" t="s">
+    <row r="22" ht="24" spans="3:4">
+      <c r="C22" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="3:4">
-      <c r="C23" s="39" t="s">
+    <row r="23" ht="24" spans="3:4">
+      <c r="C23" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" ht="69" customHeight="1" spans="3:5">
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="18"/>
+      <c r="E25" s="16"/>
     </row>
     <row r="26" ht="14.25" customHeight="1" spans="3:5">
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="18"/>
-    </row>
-    <row r="27" ht="52.2" spans="3:3">
-      <c r="C27" s="41" t="s">
+      <c r="E26" s="16"/>
+    </row>
+    <row r="27" ht="41.25" spans="3:3">
+      <c r="C27" s="31" t="s">
         <v>43</v>
       </c>
     </row>
@@ -9618,24 +9752,24 @@
   <sheetPr/>
   <dimension ref="A1:Q875"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F96" workbookViewId="0">
-      <selection activeCell="A97" sqref="$A97:$XFD97"/>
+    <sheetView tabSelected="1" topLeftCell="F56" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
   <cols>
-    <col min="4" max="4" width="22.5694444444444" customWidth="1"/>
+    <col min="4" max="4" width="22.5666666666667" customWidth="1"/>
     <col min="5" max="5" width="26.3333333333333" customWidth="1"/>
-    <col min="6" max="6" width="44.8541666666667" customWidth="1"/>
-    <col min="7" max="7" width="29.4236111111111" customWidth="1"/>
-    <col min="8" max="8" width="24.2847222222222" customWidth="1"/>
-    <col min="9" max="9" width="51.1388888888889" customWidth="1"/>
+    <col min="6" max="6" width="44.8533333333333" customWidth="1"/>
+    <col min="7" max="7" width="29.4266666666667" customWidth="1"/>
+    <col min="8" max="8" width="24.2866666666667" customWidth="1"/>
+    <col min="9" max="9" width="51.14" customWidth="1"/>
     <col min="10" max="10" width="19.6666666666667" customWidth="1"/>
     <col min="11" max="11" width="27.1666666666667" customWidth="1"/>
     <col min="13" max="13" width="33.1666666666667" customWidth="1"/>
-    <col min="14" max="14" width="23.4236111111111" customWidth="1"/>
-    <col min="15" max="15" width="29.4236111111111" customWidth="1"/>
-    <col min="16" max="16" width="29.8541666666667" customWidth="1"/>
+    <col min="14" max="14" width="23.4266666666667" customWidth="1"/>
+    <col min="15" max="15" width="29.4266666666667" customWidth="1"/>
+    <col min="16" max="16" width="29.8533333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -10554,7 +10688,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="34" ht="104.4" spans="5:17">
+    <row r="34" ht="144" spans="5:17">
       <c r="E34" t="s">
         <v>175</v>
       </c>
@@ -11188,7 +11322,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" ht="104.4" spans="5:17">
+    <row r="54" ht="144" spans="5:17">
       <c r="E54" t="s">
         <v>242</v>
       </c>
@@ -11560,7 +11694,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="66" ht="87" spans="5:17">
+    <row r="66" ht="120" spans="5:17">
       <c r="E66" t="s">
         <v>278</v>
       </c>
@@ -11602,7 +11736,7 @@
       <c r="H67" t="s">
         <v>284</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I67" s="10" t="s">
         <v>285</v>
       </c>
       <c r="N67" t="s">
@@ -12210,7 +12344,7 @@
       <c r="H86" t="s">
         <v>364</v>
       </c>
-      <c r="I86" s="10" t="s">
+      <c r="I86" s="11" t="s">
         <v>373</v>
       </c>
       <c r="N86" t="s">
@@ -12239,7 +12373,7 @@
       <c r="H87" t="s">
         <v>369</v>
       </c>
-      <c r="I87" s="11" t="s">
+      <c r="I87" s="10" t="s">
         <v>376</v>
       </c>
       <c r="N87" t="s">
@@ -12454,7 +12588,7 @@
       <c r="H94" t="s">
         <v>391</v>
       </c>
-      <c r="I94" s="10" t="s">
+      <c r="I94" s="11" t="s">
         <v>398</v>
       </c>
       <c r="N94" t="s">
@@ -12483,7 +12617,7 @@
       <c r="H95" t="s">
         <v>394</v>
       </c>
-      <c r="I95" s="11" t="s">
+      <c r="I95" s="10" t="s">
         <v>401</v>
       </c>
       <c r="N95" t="s">
@@ -12650,7 +12784,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="101" ht="104.4" spans="5:17">
+    <row r="101" ht="120" spans="5:17">
       <c r="E101" t="s">
         <v>418</v>
       </c>
@@ -12795,7 +12929,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="106" ht="139.2" spans="5:17">
+    <row r="106" ht="151.5" spans="5:17">
       <c r="E106" t="s">
         <v>433</v>
       </c>
@@ -12917,7 +13051,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="110" ht="121.8" spans="5:17">
+    <row r="110" ht="134.25" spans="5:17">
       <c r="E110" t="s">
         <v>449</v>
       </c>
@@ -13010,7 +13144,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="113" ht="139.2" spans="5:17">
+    <row r="113" ht="158.25" spans="5:17">
       <c r="E113" t="s">
         <v>459</v>
       </c>
@@ -13103,7 +13237,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="116" ht="139.2" spans="5:17">
+    <row r="116" ht="158.25" spans="5:17">
       <c r="E116" t="s">
         <v>469</v>
       </c>
@@ -13167,7 +13301,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="118" ht="121.8" spans="5:17">
+    <row r="118" ht="168" spans="5:17">
       <c r="E118" t="s">
         <v>475</v>
       </c>
@@ -13225,7 +13359,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="120" ht="121.8" spans="5:17">
+    <row r="120" ht="168" spans="5:17">
       <c r="E120" t="s">
         <v>482</v>
       </c>
@@ -13916,7 +14050,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="143" ht="156.6" spans="5:17">
+    <row r="143" ht="192" spans="5:17">
       <c r="E143" t="s">
         <v>564</v>
       </c>
@@ -13951,7 +14085,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="144" ht="243.6" spans="5:17">
+    <row r="144" ht="336" spans="5:17">
       <c r="E144" t="s">
         <v>569</v>
       </c>
@@ -13986,7 +14120,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="145" ht="243.6" spans="5:17">
+    <row r="145" ht="336" spans="5:17">
       <c r="E145" t="s">
         <v>574</v>
       </c>
@@ -14021,7 +14155,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="146" ht="243.6" spans="5:17">
+    <row r="146" ht="336" spans="5:17">
       <c r="E146" t="s">
         <v>577</v>
       </c>
@@ -14056,7 +14190,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="147" ht="243.6" spans="5:17">
+    <row r="147" ht="336" spans="5:17">
       <c r="E147" t="s">
         <v>580</v>
       </c>
@@ -14091,7 +14225,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="148" ht="208.8" spans="5:17">
+    <row r="148" ht="288" spans="5:17">
       <c r="E148" t="s">
         <v>583</v>
       </c>
@@ -14126,7 +14260,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="149" ht="208.8" spans="5:17">
+    <row r="149" ht="288" spans="5:17">
       <c r="E149" t="s">
         <v>587</v>
       </c>
@@ -14161,7 +14295,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="150" ht="34.8" spans="5:17">
+    <row r="150" ht="48" spans="5:17">
       <c r="E150" t="s">
         <v>590</v>
       </c>
@@ -14196,7 +14330,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="151" ht="34.8" spans="5:17">
+    <row r="151" ht="48" spans="5:17">
       <c r="E151" t="s">
         <v>594</v>
       </c>
@@ -27283,21 +27417,21 @@
       <selection activeCell="M182" sqref="M182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="1" width="22.4236111111111" customWidth="1"/>
-    <col min="2" max="2" width="15.4236111111111" customWidth="1"/>
-    <col min="3" max="3" width="22.7083333333333" customWidth="1"/>
-    <col min="4" max="4" width="29.4236111111111" customWidth="1"/>
+    <col min="1" max="1" width="22.4266666666667" customWidth="1"/>
+    <col min="2" max="2" width="15.4266666666667" customWidth="1"/>
+    <col min="3" max="3" width="22.7066666666667" customWidth="1"/>
+    <col min="4" max="4" width="29.4266666666667" customWidth="1"/>
     <col min="5" max="5" width="43.6666666666667" customWidth="1"/>
-    <col min="6" max="7" width="34.4236111111111" customWidth="1"/>
-    <col min="8" max="8" width="37.9166666666667" customWidth="1"/>
-    <col min="9" max="10" width="41.4166666666667" customWidth="1"/>
+    <col min="6" max="7" width="34.4266666666667" customWidth="1"/>
+    <col min="8" max="8" width="37.92" customWidth="1"/>
+    <col min="9" max="10" width="41.42" customWidth="1"/>
     <col min="11" max="11" width="16.1666666666667" customWidth="1"/>
-    <col min="12" max="12" width="29.8541666666667" customWidth="1"/>
+    <col min="12" max="12" width="29.8533333333333" customWidth="1"/>
     <col min="13" max="13" width="24.8333333333333" customWidth="1"/>
-    <col min="14" max="14" width="17.5694444444444" customWidth="1"/>
-    <col min="15" max="15" width="15.7083333333333" customWidth="1"/>
+    <col min="14" max="14" width="17.5666666666667" customWidth="1"/>
+    <col min="15" max="15" width="15.7066666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -29811,7 +29945,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="81" ht="34.8" spans="5:15">
+    <row r="81" ht="34.5" spans="5:15">
       <c r="E81" t="s">
         <v>930</v>
       </c>
@@ -29846,7 +29980,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="82" spans="5:15">
+    <row r="82" ht="24" spans="5:15">
       <c r="E82" t="s">
         <v>934</v>
       </c>
@@ -29881,7 +30015,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="83" spans="5:15">
+    <row r="83" ht="24" spans="5:15">
       <c r="E83" t="s">
         <v>937</v>
       </c>
@@ -29916,7 +30050,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="84" spans="5:15">
+    <row r="84" ht="24" spans="5:15">
       <c r="E84" t="s">
         <v>940</v>
       </c>
@@ -29951,7 +30085,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="85" spans="5:15">
+    <row r="85" ht="24" spans="5:15">
       <c r="E85" t="s">
         <v>943</v>
       </c>
@@ -29986,7 +30120,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="86" spans="5:15">
+    <row r="86" ht="24" spans="5:15">
       <c r="E86" t="s">
         <v>946</v>
       </c>
@@ -30021,7 +30155,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="87" spans="5:15">
+    <row r="87" ht="24" spans="5:15">
       <c r="E87" t="s">
         <v>949</v>
       </c>
@@ -30056,7 +30190,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="88" spans="5:15">
+    <row r="88" ht="24" spans="5:15">
       <c r="E88" t="s">
         <v>952</v>
       </c>

</xml_diff>